<commit_message>
add counter reset button + cleanup
</commit_message>
<xml_diff>
--- a/BOM_JLCSMT.xlsx
+++ b/BOM_JLCSMT.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="126">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -364,7 +364,7 @@
     <t xml:space="preserve">1k</t>
   </si>
   <si>
-    <t xml:space="preserve">R38,R37,R36,R35,R34,R33,R32,R31,R30,R29,R28,R27,R26,R25,R24,R23,R22,R21,R20,R19,R18,R17,R16,R15</t>
+    <t xml:space="preserve">R58,R38,R37,R36,R35,R34,R33,R32,R31,R30,R29,R28,R27,R26,R25,R24,R23,R22,R21,R20,R19,R18,R17,R16,R15</t>
   </si>
   <si>
     <t xml:space="preserve">C11702</t>
@@ -425,6 +425,18 @@
   </si>
   <si>
     <t xml:space="preserve">C87663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW_DIP_SPSTx01_Slide_6.7x4.1mm_W8.61mm_P2.54mm_LowProfile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW_Push_Dual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C118141</t>
   </si>
 </sst>
 </file>
@@ -651,7 +663,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="20" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1182,6 +1194,20 @@
         <v>121</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>